<commit_message>
chore: updates to ARPA output templates for 2025 Q2
</commit_message>
<xml_diff>
--- a/packages/server/src/arpa_reporter/data/treasury/project18_229233BulkUpload.xlsx
+++ b/packages/server/src/arpa_reporter/data/treasury/project18_229233BulkUpload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgu82\Desktop\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\SLFRFBulkUploadTemplates\Quarter 1 2025 Project Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1154095E-66DD-463E-A1D4-C8D9F3379E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE624F0-011C-42A2-964A-7F78D3500493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="101">
   <si>
     <t xml:space="preserve">Field ID </t>
   </si>
@@ -441,12 +441,30 @@
   <si>
     <t>Q1_2025_Expenditures__c</t>
   </si>
+  <si>
+    <t>Prog_Income_Earned_After_12_31_24__c</t>
+  </si>
+  <si>
+    <t>Total_Prog_Income_Obl_Post_Q4_2024__c</t>
+  </si>
+  <si>
+    <t>Total_Prog_Income_Exp_Post_Q4_2024__c</t>
+  </si>
+  <si>
+    <t>Program Income earned on project after December 31, 2024</t>
+  </si>
+  <si>
+    <t>Program Income obligated by deadline and reported after December 31, 2024</t>
+  </si>
+  <si>
+    <t>Program Income reported after Q4 2024 expended</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,13 +518,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -570,16 +581,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -831,7 +839,7 @@
   <dimension ref="A1:AH1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -842,8 +850,7 @@
     <col min="22" max="25" width="25.09765625" style="3" customWidth="1"/>
     <col min="26" max="26" width="28.8984375" style="3" customWidth="1"/>
     <col min="27" max="28" width="29.8984375" style="3" customWidth="1"/>
-    <col min="29" max="31" width="25.59765625" style="3" customWidth="1"/>
-    <col min="32" max="34" width="7.5" style="3" customWidth="1"/>
+    <col min="29" max="34" width="25.59765625" style="3" customWidth="1"/>
     <col min="35" max="16384" width="12.5" style="3"/>
   </cols>
   <sheetData>
@@ -924,10 +931,10 @@
       <c r="AH2" s="2"/>
     </row>
     <row r="3" spans="1:34" ht="255" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -962,396 +969,420 @@
       <c r="AH3" s="2"/>
     </row>
     <row r="4" spans="1:34" ht="66.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="S4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="6" t="s">
+      <c r="U4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="V4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="W4" s="6" t="s">
+      <c r="W4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="X4" s="6" t="s">
+      <c r="X4" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Y4" s="6" t="s">
+      <c r="Y4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="Z4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AA4" s="6" t="s">
+      <c r="AA4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AB4" s="6" t="s">
+      <c r="AB4" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AC4" s="6" t="s">
+      <c r="AC4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AD4" s="6" t="s">
+      <c r="AD4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AE4" s="6" t="s">
+      <c r="AE4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AF4" s="2"/>
-      <c r="AG4" s="2"/>
-      <c r="AH4" s="2"/>
+      <c r="AF4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AG4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="5" spans="1:34" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="N5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="R5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U5" s="6" t="s">
+      <c r="U5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V5" s="6" t="s">
+      <c r="V5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W5" s="6" t="s">
+      <c r="W5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="X5" s="6" t="s">
+      <c r="X5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="Y5" s="6" t="s">
+      <c r="Y5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Z5" s="6" t="s">
+      <c r="Z5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AA5" s="6" t="s">
+      <c r="AA5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AB5" s="6" t="s">
+      <c r="AB5" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AC5" s="6" t="s">
+      <c r="AC5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AD5" s="6" t="s">
+      <c r="AD5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AE5" s="6" t="s">
+      <c r="AE5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AF5" s="2"/>
-      <c r="AG5" s="2"/>
-      <c r="AH5" s="2"/>
+      <c r="AF5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH5" s="5" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="6" spans="1:34" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="K6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="N6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="P6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="R6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="6" t="s">
+      <c r="V6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W6" s="6" t="s">
+      <c r="W6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="X6" s="6" t="s">
+      <c r="X6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="Y6" s="6" t="s">
+      <c r="Y6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Z6" s="6" t="s">
+      <c r="Z6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AA6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AB6" s="6" t="s">
+      <c r="AB6" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AC6" s="6" t="s">
+      <c r="AC6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AD6" s="6" t="s">
+      <c r="AD6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AE6" s="6" t="s">
+      <c r="AE6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AF6" s="4"/>
-      <c r="AG6" s="4"/>
-      <c r="AH6" s="4"/>
+      <c r="AF6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG6" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH6" s="5" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:34" ht="409.6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="K7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="M7" s="5" t="s">
+      <c r="M7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="O7" s="5" t="s">
+      <c r="O7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="5" t="s">
+      <c r="S7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="T7" s="5" t="s">
+      <c r="T7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="X7" s="5" t="s">
+      <c r="X7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="Y7" s="5" t="s">
+      <c r="Y7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Z7" s="5" t="s">
+      <c r="Z7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AA7" s="5" t="s">
+      <c r="AA7" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AB7" s="5" t="s">
+      <c r="AB7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AC7" s="5" t="s">
+      <c r="AC7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AD7" s="5" t="s">
+      <c r="AD7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AE7" s="5" t="s">
+      <c r="AE7" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AF7" s="2"/>
-      <c r="AG7" s="2"/>
-      <c r="AH7" s="2"/>
+      <c r="AF7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG7" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH7" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:34" ht="43.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
@@ -1359,10 +1390,10 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
       <c r="J8" s="1"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1371,7 +1402,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="8"/>
+      <c r="R8" s="7"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
@@ -37103,9 +37134,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37326,27 +37360,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
-    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -37371,9 +37393,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D55B629F-9BAD-43E6-819F-B097A47F8C05}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44B7B1D8-F3F2-46A8-A792-B679C78EEEEB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="79f0e6e4-ac4e-4584-83f0-2cc69c4e4aae"/>
+    <ds:schemaRef ds:uri="1998147e-1bae-4425-a5b5-824e2b69f76d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>